<commit_message>
Added fix for write exception in excel: added null checking for row and cell and implemented login to create cell when required
</commit_message>
<xml_diff>
--- a/Ginger/GingerCoreNETUnitTest/TestResources/Excel/NamesWrite.xlsx
+++ b/Ginger/GingerCoreNETUnitTest/TestResources/Excel/NamesWrite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haimuz\source\MyRepos\Ginger\Ginger\GingerCoreNETUnitTest\TestResources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajdeemu\source\repos\Ginger-Automation\Ginger\Ginger\GingerCoreNETUnitTest\TestResources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FED60FF-0A93-4AAA-8F78-8F3EFF9C3E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A51A9C1-60D5-4752-9D60-86638687C911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,7 +471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -485,7 +485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -497,6 +497,11 @@
       </c>
       <c r="D5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>